<commit_message>
added a load of files
</commit_message>
<xml_diff>
--- a/Data/AGC.xlsx
+++ b/Data/AGC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Documents\My Dropbox\Work\PhD\Publications, Reports and Responsibilities\Chapters\3. Effects of invasive species on ecosystem services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Documents\My Dropbox\Work\PhD\Publications, Reports and Responsibilities\Chapters\3. Effects of invasive species on ecosystem services\Invasive_traits\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17464" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17466" uniqueCount="349">
   <si>
     <t>Related final service</t>
   </si>
@@ -1071,6 +1071,12 @@
   <si>
     <t>Spartina anglica</t>
   </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
@@ -1460,9 +1466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1481,7 +1489,7 @@
     <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -1536,8 +1544,14 @@
       <c r="R1" s="5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S1" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1596,8 +1610,14 @@
         <f>VLOOKUP(N2,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S2" s="3">
+        <v>45.663007</v>
+      </c>
+      <c r="T2" s="3">
+        <v>-84.423322999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1656,8 +1676,14 @@
         <f>VLOOKUP(N3,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S3" s="3">
+        <v>41</v>
+      </c>
+      <c r="T3" s="3">
+        <v>-117.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1716,8 +1742,14 @@
         <f>VLOOKUP(N4,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="S4" s="3">
+        <v>40.99</v>
+      </c>
+      <c r="T4" s="3">
+        <v>-117.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1776,8 +1808,14 @@
         <f>VLOOKUP(N5,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="S5" s="3">
+        <v>-13.15</v>
+      </c>
+      <c r="T5" s="3">
+        <v>130.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1836,8 +1874,14 @@
         <f>VLOOKUP(N6,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S6" s="3">
+        <v>-13.15</v>
+      </c>
+      <c r="T6" s="3">
+        <v>130.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1892,8 +1936,14 @@
         <f>VLOOKUP(N7,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S7" s="3">
+        <v>38.925229000000002</v>
+      </c>
+      <c r="T7" s="3">
+        <v>-122.412415</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1952,8 +2002,14 @@
         <f>VLOOKUP(N8,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S8" s="3">
+        <v>50.85</v>
+      </c>
+      <c r="T8" s="3">
+        <v>4.4166670000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -2012,8 +2068,14 @@
         <f>VLOOKUP(N9,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S9" s="3">
+        <v>50.865777999999999</v>
+      </c>
+      <c r="T9" s="3">
+        <v>4.4693759999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -2072,8 +2134,14 @@
         <f>VLOOKUP(N10,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S10" s="3">
+        <v>50.453569000000002</v>
+      </c>
+      <c r="T10" s="3">
+        <v>3.8191220000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2132,8 +2200,14 @@
         <f>VLOOKUP(N11,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S11" s="3">
+        <v>40.136333329999999</v>
+      </c>
+      <c r="T11" s="3">
+        <v>-120.0731667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -2188,8 +2262,14 @@
         <f>VLOOKUP(N12,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="S12" s="3">
+        <v>46.916666669999998</v>
+      </c>
+      <c r="T12" s="3">
+        <v>-123.2666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2248,8 +2328,14 @@
         <f>VLOOKUP(N13,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S13" s="3">
+        <v>25.995080999999999</v>
+      </c>
+      <c r="T13" s="3">
+        <v>-81.482849000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -2308,8 +2394,14 @@
         <f>VLOOKUP(N14,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S14" s="3">
+        <v>43.583333330000002</v>
+      </c>
+      <c r="T14" s="3">
+        <v>-102.6333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2368,8 +2460,14 @@
         <f>VLOOKUP(N15,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S15" s="3">
+        <v>43.583333330000002</v>
+      </c>
+      <c r="T15" s="3">
+        <v>-102.6333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -2428,8 +2526,14 @@
         <f>VLOOKUP(N16,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S16" s="3">
+        <v>43.583333330000002</v>
+      </c>
+      <c r="T16" s="3">
+        <v>-102.6333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -2488,8 +2592,14 @@
         <f>VLOOKUP(N17,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S17" s="3">
+        <v>43.583333330000002</v>
+      </c>
+      <c r="T17" s="3">
+        <v>-102.6333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2548,8 +2658,14 @@
         <f>VLOOKUP(N18,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S18" s="3">
+        <v>33.380000000000003</v>
+      </c>
+      <c r="T18" s="3">
+        <v>-117.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2608,8 +2724,14 @@
         <f>VLOOKUP(N19,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S19" s="3">
+        <v>50.895426999999998</v>
+      </c>
+      <c r="T19" s="3">
+        <v>4.416804</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -2668,8 +2790,14 @@
         <f>VLOOKUP(N20,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>1.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S20" s="3">
+        <v>50.755789999999998</v>
+      </c>
+      <c r="T20" s="3">
+        <v>-120.46577499999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2728,8 +2856,14 @@
         <f>VLOOKUP(N21,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S21" s="3">
+        <v>50.799751000000001</v>
+      </c>
+      <c r="T21" s="3">
+        <v>4.4146159999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -2788,8 +2922,14 @@
         <f>VLOOKUP(N22,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S22" s="3">
+        <v>40.57</v>
+      </c>
+      <c r="T22" s="3">
+        <v>-118.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -2848,8 +2988,14 @@
         <f>VLOOKUP(N23,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="S23" s="3">
+        <v>50.862771000000002</v>
+      </c>
+      <c r="T23" s="3">
+        <v>4.4709630000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2908,8 +3054,14 @@
         <f>VLOOKUP(N24,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>1.0668</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S24" s="3">
+        <v>19.768055555555556</v>
+      </c>
+      <c r="T24" s="3">
+        <v>-155.93861111111113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -2968,8 +3120,14 @@
         <f>VLOOKUP(N25,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S25" s="3">
+        <v>39.133333333333333</v>
+      </c>
+      <c r="T25" s="3">
+        <v>26.516666666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -3028,8 +3186,14 @@
         <f>VLOOKUP(N26,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>1.0668</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S26" s="3">
+        <v>31.15</v>
+      </c>
+      <c r="T26" s="3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
@@ -3088,8 +3252,14 @@
         <f>VLOOKUP(N27,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>1.0668</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S27" s="3">
+        <v>31.416666666666668</v>
+      </c>
+      <c r="T27" s="3">
+        <v>121.83333333333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -3148,8 +3318,14 @@
         <f>VLOOKUP(N28,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S28" s="3">
+        <v>42.350045000000001</v>
+      </c>
+      <c r="T28" s="3">
+        <v>-72.523111999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
@@ -3208,8 +3384,14 @@
         <f>VLOOKUP(N29,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S29" s="3">
+        <v>47.4</v>
+      </c>
+      <c r="T29" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
@@ -3268,8 +3450,14 @@
         <f>VLOOKUP(N30,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S30" s="3">
+        <v>42.320954</v>
+      </c>
+      <c r="T30" s="3">
+        <v>-72.590102999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3328,8 +3516,14 @@
         <f>VLOOKUP(N31,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S31" s="3">
+        <v>40.013888889999997</v>
+      </c>
+      <c r="T31" s="3">
+        <v>-105.2055556</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>17</v>
       </c>
@@ -3388,8 +3582,14 @@
         <f>VLOOKUP(N32,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="S32" s="3">
+        <v>42.291722999999998</v>
+      </c>
+      <c r="T32" s="3">
+        <v>-72.617740999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
@@ -3448,8 +3648,14 @@
         <f>VLOOKUP(N33,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>0.60960000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S33" s="3">
+        <v>49.366666666666667</v>
+      </c>
+      <c r="T33" s="3">
+        <v>-107.883333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
@@ -3508,8 +3714,14 @@
         <f>VLOOKUP(N34,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S34" s="3">
+        <v>47.4</v>
+      </c>
+      <c r="T34" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>17</v>
       </c>
@@ -3568,8 +3780,14 @@
         <f>VLOOKUP(N35,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>2.4993599999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S35" s="3">
+        <v>47.4</v>
+      </c>
+      <c r="T35" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>17</v>
       </c>
@@ -3628,8 +3846,14 @@
         <f>VLOOKUP(N36,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>1.238</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S36" s="3">
+        <v>41.616666666666667</v>
+      </c>
+      <c r="T36" s="3">
+        <v>-83.233333333333334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -3687,6 +3911,12 @@
       <c r="R37">
         <f>VLOOKUP(N37,Height!$B$2:$N$2062,13,FALSE)</f>
         <v>1.238</v>
+      </c>
+      <c r="S37" s="3">
+        <v>41.616666666666667</v>
+      </c>
+      <c r="T37" s="3">
+        <v>-83.233333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>